<commit_message>
CodeElements tests for ambiguous first tokens OK
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Code elements.xlsx
+++ b/TypeCobol/Documentation/Studies/Code elements.xlsx
@@ -780,9 +780,6 @@
     <t>blankWhenZeroClause</t>
   </si>
   <si>
-    <t>blankWhenZeroClause, xmlGenerateStatement + whenSearchCondition, whenEvaluateCondition, whenOtherCondition</t>
-  </si>
-  <si>
     <t>XML GENERATE
 XML PARSE</t>
   </si>
@@ -857,7 +854,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>whenSearchCondition
+      <t>whenConditionalExpression
 whenEvaluateCondition</t>
     </r>
     <r>
@@ -871,6 +868,9 @@
       <t xml:space="preserve">
 whenOtherCondition</t>
     </r>
+  </si>
+  <si>
+    <t>blankWhenZeroClause, xmlGenerateStatement + whenConditionalExpression, whenEvaluateCondition, whenOtherCondition</t>
   </si>
 </sst>
 </file>
@@ -1244,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1333,7 @@
         <v>168</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>168</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1545,12 +1545,12 @@
         <v>168</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>181</v>
@@ -1947,7 +1947,7 @@
         <v>168</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
     </row>
     <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>188</v>
@@ -2060,7 +2060,7 @@
         <v>168</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2091,7 +2091,7 @@
         <v>168</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2142,7 +2142,7 @@
         <v>168</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2159,7 +2159,7 @@
         <v>196</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2176,7 +2176,7 @@
         <v>196</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
         <v>168</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2306,7 +2306,7 @@
         <v>168</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2323,7 +2323,7 @@
         <v>168</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2374,7 +2374,7 @@
         <v>168</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2436,7 +2436,7 @@
         <v>168</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2577,7 +2577,7 @@
         <v>168</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2594,7 +2594,7 @@
         <v>168</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2645,7 +2645,7 @@
         <v>168</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2662,7 +2662,7 @@
         <v>168</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2696,7 +2696,7 @@
         <v>168</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2761,7 +2761,7 @@
         <v>168</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2778,7 +2778,7 @@
         <v>168</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2880,7 +2880,7 @@
         <v>168</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2902,13 +2902,13 @@
         <v>233</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>234</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2925,7 +2925,7 @@
         <v>168</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2947,16 +2947,16 @@
     </row>
     <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="C104" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D104" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>238</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>170</v>

</xml_diff>